<commit_message>
(WB): Update warehouse mapping table
</commit_message>
<xml_diff>
--- a/wb/scripts/wb_warehouses_mapping.xlsx
+++ b/wb/scripts/wb_warehouses_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\artem\work\1Bit\Задачи\Выгрузка по API WB\develop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Artem\work\1Bit\Задачи\Маркетплейсы\wb\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89936003-DCFE-404B-BD5D-48B95286F79F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80816602-7262-40BF-8293-863D5219ABCD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Монопалеты" sheetId="3" r:id="rId1"/>
@@ -24,23 +24,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Монопалеты!$A$1:$E$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Новые склады'!$A$1:$J$33</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="135">
   <si>
     <t>Обухово СГТ</t>
   </si>
@@ -433,6 +427,18 @@
   </si>
   <si>
     <t>Ювелирка_Монопалеты</t>
+  </si>
+  <si>
+    <t>СЦ Оренбург центральная</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург Уткина Заводь МП</t>
+  </si>
+  <si>
+    <t>Сарапул</t>
+  </si>
+  <si>
+    <t>СЦ Ереван</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -737,13 +743,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{8BBDD975-95AF-4FE7-89A7-F4D6C59D03D9}"/>
     <cellStyle name="Обычный 3" xfId="2" xr:uid="{02310D06-DCB8-4D11-B6DB-FB78F6908624}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1024,10 +1054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1005EDC7-16BB-4C00-8912-E9DF3BE8406E}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,11 +1570,11 @@
       <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>17</v>
+      <c r="B30" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>0</v>
@@ -1557,13 +1588,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>17</v>
@@ -1574,13 +1605,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>17</v>
@@ -1591,13 +1622,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>17</v>
@@ -1608,13 +1639,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>17</v>
@@ -1625,7 +1656,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>17</v>
@@ -1642,7 +1673,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>17</v>
@@ -1658,13 +1689,13 @@
       <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>92</v>
+      <c r="B37" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="11" t="s">
@@ -1676,13 +1707,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>17</v>
@@ -1693,13 +1724,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>17</v>
@@ -1710,7 +1741,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>17</v>
@@ -1727,16 +1758,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,16 +1775,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1761,13 +1792,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>17</v>
@@ -1777,51 +1808,51 @@
       <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>14</v>
+      <c r="B44" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>8</v>
+      <c r="B45" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>22</v>
+      <c r="B46" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1829,7 +1860,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>14</v>
@@ -1846,13 +1877,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>14</v>
@@ -1863,7 +1894,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>14</v>
@@ -1881,7 +1912,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>14</v>
@@ -1898,7 +1929,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>14</v>
@@ -1915,7 +1946,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>14</v>
@@ -1932,9 +1963,9 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C53" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="10" t="s">
@@ -1949,13 +1980,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>14</v>
@@ -1966,9 +1997,9 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="10" t="s">
@@ -1982,14 +2013,14 @@
       <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>3</v>
+      <c r="B56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>14</v>
@@ -2000,16 +2031,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2017,33 +2048,33 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>1</v>
+      <c r="B59" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>3</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2051,13 +2082,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>12</v>
@@ -2068,7 +2099,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>12</v>
@@ -2084,14 +2115,14 @@
       <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>82</v>
+      <c r="B62" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>12</v>
@@ -2101,14 +2132,14 @@
       <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>99</v>
+      <c r="B63" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>111</v>
+        <v>3</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>12</v>
@@ -2118,14 +2149,14 @@
       <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>100</v>
+      <c r="B64" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>12</v>
@@ -2135,34 +2166,34 @@
       <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>29</v>
+      <c r="B65" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>35</v>
+      <c r="B66" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2170,16 +2201,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2187,29 +2218,29 @@
         <v>67</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D68" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>95</v>
+      <c r="B69" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="D69" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E69" s="11" t="s">
@@ -2220,30 +2251,30 @@
       <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>88</v>
+      <c r="B70" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71" s="21" t="s">
-        <v>18</v>
+      <c r="B71" s="27" t="s">
+        <v>79</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="17" t="s">
         <v>1</v>
       </c>
       <c r="E71" s="11" t="s">
@@ -2254,13 +2285,13 @@
       <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72" s="21" t="s">
-        <v>41</v>
+      <c r="B72" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="17" t="s">
         <v>1</v>
       </c>
       <c r="E72" s="11" t="s">
@@ -2272,10 +2303,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>1</v>
@@ -2288,17 +2319,17 @@
       <c r="A74" s="3">
         <v>73</v>
       </c>
-      <c r="B74" s="21" t="s">
-        <v>42</v>
+      <c r="B74" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2306,13 +2337,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>14</v>
@@ -2322,14 +2353,14 @@
       <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76" s="24" t="s">
-        <v>121</v>
+      <c r="B76" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>14</v>
@@ -2339,14 +2370,14 @@
       <c r="A77" s="3">
         <v>76</v>
       </c>
-      <c r="B77" s="21" t="s">
-        <v>33</v>
+      <c r="B77" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>14</v>
@@ -2357,7 +2388,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>36</v>
@@ -2373,14 +2404,14 @@
       <c r="A79" s="3">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
-        <v>96</v>
-      </c>
-      <c r="C79" s="8" t="s">
+      <c r="B79" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D79" s="15" t="s">
-        <v>3</v>
+      <c r="C79" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>14</v>
@@ -2390,51 +2421,51 @@
       <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>0</v>
+      <c r="B80" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>0</v>
+      <c r="B81" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D81" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
-        <v>103</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>0</v>
+      <c r="B82" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2442,16 +2473,16 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2459,81 +2490,81 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="B85" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>3</v>
+      <c r="B85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>0</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>85</v>
       </c>
-      <c r="B86" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D86" s="16" t="s">
-        <v>3</v>
+      <c r="B86" t="s">
+        <v>103</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>0</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>86</v>
       </c>
-      <c r="B87" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C87" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D87" s="16" t="s">
-        <v>3</v>
+      <c r="B87" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>87</v>
       </c>
-      <c r="B88" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>3</v>
+      <c r="B88" t="s">
+        <v>83</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>14</v>
@@ -2544,7 +2575,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>39</v>
@@ -2561,7 +2592,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>39</v>
@@ -2578,13 +2609,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C91" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>14</v>
@@ -2594,8 +2625,8 @@
       <c r="A92" s="3">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
-        <v>122</v>
+      <c r="B92" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="C92" s="16" t="s">
         <v>39</v>
@@ -2611,48 +2642,48 @@
       <c r="A93" s="3">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
-        <v>78</v>
+      <c r="B93" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="15" t="s">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>93</v>
       </c>
-      <c r="B94" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C94" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="20" t="s">
-        <v>17</v>
+      <c r="B94" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>94</v>
       </c>
-      <c r="B95" t="s">
-        <v>87</v>
+      <c r="B95" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>111</v>
+        <v>39</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>14</v>
@@ -2663,13 +2694,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>89</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>14</v>
@@ -2680,13 +2711,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="C97" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>111</v>
+        <v>39</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>14</v>
@@ -2697,47 +2728,47 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
-        <v>94</v>
-      </c>
-      <c r="C99" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E99" s="11" t="s">
-        <v>14</v>
+      <c r="B99" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C99" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>99</v>
       </c>
-      <c r="B100" s="21" t="s">
-        <v>7</v>
+      <c r="B100" t="s">
+        <v>87</v>
       </c>
       <c r="C100" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="16" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>14</v>
@@ -2747,14 +2778,14 @@
       <c r="A101" s="3">
         <v>100</v>
       </c>
-      <c r="B101" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C101" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>0</v>
+      <c r="B101" t="s">
+        <v>89</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>14</v>
@@ -2764,14 +2795,14 @@
       <c r="A102" s="3">
         <v>101</v>
       </c>
-      <c r="B102" s="21" t="s">
-        <v>37</v>
+      <c r="B102" t="s">
+        <v>91</v>
       </c>
       <c r="C102" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>14</v>
@@ -2781,14 +2812,14 @@
       <c r="A103" s="3">
         <v>102</v>
       </c>
-      <c r="B103" s="21" t="s">
-        <v>28</v>
+      <c r="B103" t="s">
+        <v>93</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>14</v>
@@ -2798,14 +2829,14 @@
       <c r="A104" s="3">
         <v>103</v>
       </c>
-      <c r="B104" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>0</v>
+      <c r="B104" t="s">
+        <v>94</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>14</v>
@@ -2816,7 +2847,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C105" s="16" t="s">
         <v>7</v>
@@ -2833,7 +2864,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C106" s="16" t="s">
         <v>7</v>
@@ -2849,8 +2880,8 @@
       <c r="A107" s="3">
         <v>106</v>
       </c>
-      <c r="B107" s="25" t="s">
-        <v>124</v>
+      <c r="B107" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>7</v>
@@ -2862,16 +2893,104 @@
         <v>14</v>
       </c>
     </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>107</v>
+      </c>
+      <c r="B108" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="3">
+        <v>108</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>109</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>110</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="3">
+        <v>111</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E70" xr:uid="{39E07448-53B2-40B2-84E0-B8961ECA3970}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E107">
+    <sortState ref="A2:E112">
       <sortCondition ref="C1:C70"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
+  <sortState ref="A2:E70">
     <sortCondition ref="A2:A70"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2879,10 +2998,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DADA36-D357-46A6-883A-34D12081D050}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3426,14 +3546,14 @@
       <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>17</v>
+      <c r="B32" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>17</v>
@@ -3444,12 +3564,12 @@
         <v>32</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -3460,13 +3580,13 @@
       <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>105</v>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
@@ -3478,12 +3598,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E35" s="11" t="s">
@@ -3494,51 +3614,51 @@
       <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>14</v>
+      <c r="B36" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>0</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>14</v>
+      <c r="B37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>22</v>
+      <c r="B38" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>0</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -3546,7 +3666,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>14</v>
@@ -3563,13 +3683,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>14</v>
@@ -3580,7 +3700,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>14</v>
@@ -3597,9 +3717,9 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="6" t="s">
@@ -3614,13 +3734,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>14</v>
@@ -3631,13 +3751,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>14</v>
@@ -3648,9 +3768,9 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -3665,7 +3785,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>14</v>
@@ -3682,13 +3802,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>14</v>
@@ -3698,13 +3818,13 @@
       <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>79</v>
+      <c r="B48" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -3715,13 +3835,13 @@
       <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>90</v>
+      <c r="B49" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E49" s="11" t="s">
@@ -3732,13 +3852,13 @@
       <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="12" t="s">
+      <c r="B50" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E50" s="11" t="s">
@@ -3750,13 +3870,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>14</v>
@@ -3766,51 +3886,51 @@
       <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>12</v>
+      <c r="B52" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>10</v>
+      <c r="B53" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>34</v>
+      <c r="B54" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -3818,7 +3938,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>12</v>
@@ -3835,7 +3955,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>12</v>
@@ -3851,13 +3971,13 @@
       <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>82</v>
+      <c r="B57" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E57" s="11" t="s">
@@ -3868,13 +3988,13 @@
       <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>84</v>
+      <c r="B58" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="11" t="s">
@@ -3885,13 +4005,13 @@
       <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>85</v>
+      <c r="B59" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E59" s="11" t="s">
@@ -3903,7 +4023,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>12</v>
@@ -3920,7 +4040,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>12</v>
@@ -3937,7 +4057,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>12</v>
@@ -3953,68 +4073,68 @@
       <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>23</v>
+      <c r="B63" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>32</v>
+      <c r="B64" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>59</v>
+      <c r="B65" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>0</v>
+      <c r="B66" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -4022,7 +4142,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C67" s="17" t="s">
         <v>23</v>
@@ -4039,7 +4159,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C68" s="17" t="s">
         <v>23</v>
@@ -4055,13 +4175,13 @@
       <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>81</v>
+      <c r="B69" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E69" s="11" t="s">
@@ -4072,13 +4192,13 @@
       <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>97</v>
+      <c r="B70" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E70" s="11" t="s">
@@ -4089,13 +4209,13 @@
       <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71" s="27" t="s">
-        <v>103</v>
+      <c r="B71" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D71" s="17" t="s">
+      <c r="D71" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E71" s="11" t="s">
@@ -4106,14 +4226,14 @@
       <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72" s="27" t="s">
-        <v>106</v>
+      <c r="B72" s="21" t="s">
+        <v>72</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="17" t="s">
-        <v>1</v>
+      <c r="D72" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>17</v>
@@ -4123,17 +4243,17 @@
       <c r="A73" s="3">
         <v>72</v>
       </c>
-      <c r="B73" s="21" t="s">
-        <v>18</v>
+      <c r="B73" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>0</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -4141,50 +4261,50 @@
         <v>73</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
-      <c r="B75" s="21" t="s">
-        <v>20</v>
+      <c r="B75" s="27" t="s">
+        <v>103</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D75" s="16" t="s">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>0</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76" s="21" t="s">
-        <v>46</v>
+      <c r="B76" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D76" s="16" t="s">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -4192,13 +4312,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>14</v>
@@ -4208,14 +4328,14 @@
       <c r="A78" s="3">
         <v>77</v>
       </c>
-      <c r="B78" s="21" t="s">
-        <v>50</v>
+      <c r="B78" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D78" s="16" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>14</v>
@@ -4226,7 +4346,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>20</v>
@@ -4242,13 +4362,13 @@
       <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
-        <v>96</v>
-      </c>
-      <c r="C80" s="15" t="s">
+      <c r="B80" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E80" s="11" t="s">
@@ -4259,13 +4379,13 @@
       <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
-        <v>98</v>
-      </c>
-      <c r="C81" s="15" t="s">
+      <c r="B81" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E81" s="11" t="s">
@@ -4276,8 +4396,8 @@
       <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
-        <v>122</v>
+      <c r="B82" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>20</v>
@@ -4293,48 +4413,48 @@
       <c r="A83" s="3">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
-        <v>78</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="15" t="s">
-        <v>0</v>
+      <c r="B83" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>83</v>
       </c>
-      <c r="B84" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>17</v>
+      <c r="B84" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="B85" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>1</v>
+      <c r="B85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>14</v>
@@ -4344,14 +4464,14 @@
       <c r="A86" s="3">
         <v>85</v>
       </c>
-      <c r="B86" s="23" t="s">
-        <v>13</v>
+      <c r="B86" t="s">
+        <v>122</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>14</v>
@@ -4361,14 +4481,14 @@
       <c r="A87" s="3">
         <v>86</v>
       </c>
-      <c r="B87" s="21" t="s">
-        <v>53</v>
+      <c r="B87" t="s">
+        <v>132</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>14</v>
@@ -4379,46 +4499,46 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>88</v>
       </c>
-      <c r="B89" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D89" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>14</v>
+      <c r="B89" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>89</v>
       </c>
-      <c r="B90" t="s">
-        <v>91</v>
-      </c>
-      <c r="C90" s="16" t="s">
+      <c r="B90" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D90" s="15" t="s">
+      <c r="D90" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E90" s="11" t="s">
@@ -4429,13 +4549,13 @@
       <c r="A91" s="3">
         <v>90</v>
       </c>
-      <c r="B91" t="s">
-        <v>93</v>
+      <c r="B91" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="C91" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D91" s="15" t="s">
+      <c r="D91" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E91" s="11" t="s">
@@ -4446,13 +4566,13 @@
       <c r="A92" s="3">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
-        <v>94</v>
-      </c>
-      <c r="C92" s="15" t="s">
+      <c r="B92" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C92" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E92" s="11" t="s">
@@ -4463,14 +4583,14 @@
       <c r="A93" s="3">
         <v>92</v>
       </c>
-      <c r="B93" s="21" t="s">
-        <v>7</v>
+      <c r="B93" t="s">
+        <v>87</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" s="16" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>14</v>
@@ -4480,14 +4600,14 @@
       <c r="A94" s="3">
         <v>93</v>
       </c>
-      <c r="B94" s="21" t="s">
-        <v>26</v>
+      <c r="B94" t="s">
+        <v>89</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E94" s="11" t="s">
         <v>14</v>
@@ -4497,13 +4617,13 @@
       <c r="A95" s="3">
         <v>94</v>
       </c>
-      <c r="B95" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C95" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" s="16" t="s">
+      <c r="B95" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="15" t="s">
         <v>1</v>
       </c>
       <c r="E95" s="11" t="s">
@@ -4514,14 +4634,14 @@
       <c r="A96" s="3">
         <v>95</v>
       </c>
-      <c r="B96" s="21" t="s">
-        <v>42</v>
+      <c r="B96" t="s">
+        <v>93</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D96" s="16" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>14</v>
@@ -4531,14 +4651,14 @@
       <c r="A97" s="3">
         <v>96</v>
       </c>
-      <c r="B97" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C97" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D97" s="16" t="s">
-        <v>0</v>
+      <c r="B97" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>14</v>
@@ -4549,7 +4669,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C98" s="17" t="s">
         <v>7</v>
@@ -4565,14 +4685,14 @@
       <c r="A99" s="3">
         <v>98</v>
       </c>
-      <c r="B99" s="24" t="s">
-        <v>121</v>
+      <c r="B99" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="C99" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>14</v>
@@ -4583,13 +4703,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C100" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>14</v>
@@ -4600,13 +4720,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C101" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>14</v>
@@ -4617,13 +4737,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C102" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>14</v>
@@ -4634,7 +4754,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C103" s="17" t="s">
         <v>7</v>
@@ -4650,14 +4770,14 @@
       <c r="A104" s="3">
         <v>103</v>
       </c>
-      <c r="B104" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C104" s="16" t="s">
+      <c r="B104" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C104" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>14</v>
@@ -4668,7 +4788,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C105" s="17" t="s">
         <v>7</v>
@@ -4686,7 +4806,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="C106" s="17" t="s">
         <v>7</v>
@@ -4703,38 +4823,126 @@
       <c r="A107" s="3">
         <v>106</v>
       </c>
-      <c r="B107" s="25" t="s">
-        <v>124</v>
+      <c r="B107" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E107" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>107</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="3">
+        <v>108</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>109</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E110" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>110</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="3">
+        <v>111</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="32" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E70" xr:uid="{C090F888-E92F-4062-A7BF-EACE1BB87CF6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E107">
+    <sortState ref="A2:E112">
       <sortCondition ref="C1:C70"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
+  <sortState ref="A2:E70">
     <sortCondition ref="A2:A70"/>
   </sortState>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EBA4D3-E27E-4A20-AFD9-2556285A3AB8}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5959,6 +6167,153 @@
         <v>45805</v>
       </c>
     </row>
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="41"/>
+      <c r="F40" s="42"/>
+      <c r="G40" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="31">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>132</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="31">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="31">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="31">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="31">
+        <v>45882</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J33" xr:uid="{5A56123C-ACF9-40DA-8C18-A8E6EC1A6352}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5970,8 +6325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F973164-6FF0-460D-9814-D9364B7B51EF}">
   <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6219,7 +6574,7 @@
   <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>